<commit_message>
Fix .gitignore to allow pushing excel template
</commit_message>
<xml_diff>
--- a/scenarios/receptionist.xlsx
+++ b/scenarios/receptionist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\robocup\data-generator\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DE260F-0C44-4162-9361-3B83B0DE0626}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FB730B-1C96-4782-AD92-2D5B6CD32ED8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,8 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>0.1</v>
+        <f>E2+1</f>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1032,7 +1033,8 @@
         <v>13</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <f t="shared" ref="E4:E52" si="1">E3+1</f>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1050,7 +1052,8 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1074,7 +1077,8 @@
         <v>14</v>
       </c>
       <c r="E6">
-        <v>0.4</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1092,7 +1096,8 @@
         <v>15</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="F7" s="4">
         <v>40</v>
@@ -1111,7 +1116,8 @@
         <v>16</v>
       </c>
       <c r="E8">
-        <v>1.1000000000000001</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1135,7 +1141,8 @@
         <v>18</v>
       </c>
       <c r="E9">
-        <v>1.2</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1160,7 +1167,8 @@
         <v>20</v>
       </c>
       <c r="E10">
-        <v>1.3</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1197,7 +1205,8 @@
         <v>22</v>
       </c>
       <c r="E11">
-        <v>1.4</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1222,7 +1231,8 @@
         <v>24</v>
       </c>
       <c r="E12" s="4">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="F12" s="4">
         <v>30</v>
@@ -1241,7 +1251,8 @@
         <v>25</v>
       </c>
       <c r="E13">
-        <v>2.1</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1272,7 +1283,8 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>2.2000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1296,7 +1308,8 @@
         <v>28</v>
       </c>
       <c r="E15" s="4">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="F15" s="4">
         <v>10</v>
@@ -1315,7 +1328,8 @@
         <v>30</v>
       </c>
       <c r="E16">
-        <v>3.1</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1340,7 +1354,8 @@
         <v>31</v>
       </c>
       <c r="E17">
-        <v>3.2</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1372,7 +1387,8 @@
         <v>32</v>
       </c>
       <c r="E18" s="4">
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="F18" s="4">
         <v>10</v>
@@ -1391,7 +1407,8 @@
         <v>30</v>
       </c>
       <c r="E19">
-        <v>4.0999999999999996</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1416,7 +1433,8 @@
         <v>31</v>
       </c>
       <c r="E20">
-        <v>4.2</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1448,7 +1466,8 @@
         <v>33</v>
       </c>
       <c r="E21" s="4">
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="F21" s="4">
         <v>20</v>
@@ -1467,7 +1486,8 @@
         <v>35</v>
       </c>
       <c r="E22">
-        <v>5.0999999999999996</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1491,7 +1511,8 @@
         <v>36</v>
       </c>
       <c r="E23">
-        <v>5.2</v>
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1515,7 +1536,8 @@
         <v>37</v>
       </c>
       <c r="E24">
-        <v>5.3</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1540,7 +1562,8 @@
         <v>38</v>
       </c>
       <c r="E25" s="4">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
       <c r="F25" s="4">
         <v>20</v>
@@ -1559,7 +1582,8 @@
         <v>24</v>
       </c>
       <c r="E26">
-        <v>6.1</v>
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1583,7 +1607,8 @@
         <v>39</v>
       </c>
       <c r="E27" s="4">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="F27" s="4">
         <v>20</v>
@@ -1595,14 +1620,15 @@
     </row>
     <row r="28" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" ref="A28:A52" si="1">A27+F28</f>
+        <f t="shared" ref="A28:A52" si="2">A27+F28</f>
         <v>170</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
       <c r="E28">
-        <v>7.1</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1619,14 +1645,15 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
       </c>
       <c r="E29">
-        <v>7.2</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1637,14 +1664,15 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
       <c r="E30">
-        <v>7.3</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1661,14 +1689,15 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
       </c>
       <c r="E31">
-        <v>7.4</v>
+        <f t="shared" si="1"/>
+        <v>29</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1679,14 +1708,15 @@
     </row>
     <row r="32" spans="1:11" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="4">
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="F32" s="4">
         <v>40</v>
@@ -1698,14 +1728,15 @@
     </row>
     <row r="33" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="D33" t="s">
         <v>16</v>
       </c>
       <c r="E33">
-        <v>8.1</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1722,14 +1753,15 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="D34" t="s">
         <v>18</v>
       </c>
       <c r="E34">
-        <v>8.1999999999999993</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1747,14 +1779,15 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="D35" t="s">
         <v>20</v>
       </c>
       <c r="E35">
-        <v>8.3000000000000007</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1778,14 +1811,15 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
       </c>
       <c r="E36">
-        <v>8.4</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1803,14 +1837,15 @@
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E37" s="4">
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="F37" s="4">
         <v>30</v>
@@ -1822,14 +1857,15 @@
     </row>
     <row r="38" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="D38" t="s">
         <v>25</v>
       </c>
       <c r="E38">
-        <v>9.1</v>
+        <f t="shared" si="1"/>
+        <v>36</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1853,14 +1889,15 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="D39" t="s">
         <v>24</v>
       </c>
       <c r="E39">
-        <v>9.1999999999999993</v>
+        <f t="shared" si="1"/>
+        <v>37</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1877,14 +1914,15 @@
     </row>
     <row r="40" spans="1:11" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E40" s="4">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
       <c r="F40" s="4">
         <v>10</v>
@@ -1896,14 +1934,15 @@
     </row>
     <row r="41" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="D41" t="s">
         <v>42</v>
       </c>
       <c r="E41">
-        <v>10.1</v>
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1921,14 +1960,15 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="D42" t="s">
         <v>31</v>
       </c>
       <c r="E42">
-        <v>10.199999999999999</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1953,14 +1993,15 @@
     </row>
     <row r="43" spans="1:11" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E43" s="4">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>41</v>
       </c>
       <c r="F43" s="4">
         <v>10</v>
@@ -1972,14 +2013,15 @@
     </row>
     <row r="44" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260</v>
       </c>
       <c r="D44" t="s">
         <v>65</v>
       </c>
       <c r="E44">
-        <v>11.1</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -1997,14 +2039,15 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260</v>
       </c>
       <c r="D45" t="s">
         <v>31</v>
       </c>
       <c r="E45">
-        <v>11.2</v>
+        <f t="shared" si="1"/>
+        <v>43</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -2029,14 +2072,15 @@
     </row>
     <row r="46" spans="1:11" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>270</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>44</v>
       </c>
       <c r="E46" s="4">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="F46" s="4">
         <v>10</v>
@@ -2048,14 +2092,15 @@
     </row>
     <row r="47" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>270</v>
       </c>
       <c r="D47" t="s">
         <v>30</v>
       </c>
       <c r="E47">
-        <v>12.1</v>
+        <f t="shared" si="1"/>
+        <v>45</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -2073,14 +2118,15 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>270</v>
       </c>
       <c r="D48" t="s">
         <v>31</v>
       </c>
       <c r="E48">
-        <v>12.2</v>
+        <f t="shared" si="1"/>
+        <v>46</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -2105,14 +2151,15 @@
     </row>
     <row r="49" spans="1:11" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E49" s="4">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>47</v>
       </c>
       <c r="F49" s="4">
         <v>30</v>
@@ -2124,14 +2171,15 @@
     </row>
     <row r="50" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="D50" t="s">
         <v>35</v>
       </c>
       <c r="E50">
-        <v>13.1</v>
+        <f t="shared" si="1"/>
+        <v>48</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -2148,14 +2196,15 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="D51" t="s">
         <v>36</v>
       </c>
       <c r="E51">
-        <v>13.2</v>
+        <f t="shared" si="1"/>
+        <v>49</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2172,14 +2221,15 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="D52" t="s">
         <v>37</v>
       </c>
       <c r="E52">
-        <v>13.3</v>
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -2191,8 +2241,8 @@
         <v>56</v>
       </c>
       <c r="I52" s="2" t="str">
-        <f>guest1</f>
-        <v>Guest 1</v>
+        <f>guest2</f>
+        <v>Guest 2</v>
       </c>
     </row>
   </sheetData>
@@ -2221,7 +2271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -2251,7 +2301,7 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>IF(ISBLANK(Steps!E3), "", Steps!E3)</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2260,7 +2310,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>IF(ISBLANK(Steps!E4), "", Steps!E4)</f>
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2269,7 +2319,7 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>IF(ISBLANK(Steps!E5), "", Steps!E5)</f>
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -2278,7 +2328,7 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>IF(ISBLANK(Steps!E6), "", Steps!E6)</f>
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -2287,7 +2337,7 @@
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>IF(ISBLANK(Steps!E7), "", Steps!E7)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -2296,7 +2346,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>IF(ISBLANK(Steps!E8), "", Steps!E8)</f>
-        <v>1.1000000000000001</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -2305,7 +2355,7 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>IF(ISBLANK(Steps!E9), "", Steps!E9)</f>
-        <v>1.2</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -2314,7 +2364,7 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>IF(ISBLANK(Steps!E10), "", Steps!E10)</f>
-        <v>1.3</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -2323,7 +2373,7 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>IF(ISBLANK(Steps!E11), "", Steps!E11)</f>
-        <v>1.4</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -2332,7 +2382,7 @@
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>IF(ISBLANK(Steps!E12), "", Steps!E12)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2341,7 +2391,7 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>IF(ISBLANK(Steps!E13), "", Steps!E13)</f>
-        <v>2.1</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2350,7 +2400,7 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>IF(ISBLANK(Steps!E14), "", Steps!E14)</f>
-        <v>2.2000000000000002</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2359,7 +2409,7 @@
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>IF(ISBLANK(Steps!E15), "", Steps!E15)</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -2368,7 +2418,7 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>IF(ISBLANK(Steps!E16), "", Steps!E16)</f>
-        <v>3.1</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2377,7 +2427,7 @@
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>IF(ISBLANK(Steps!E17), "", Steps!E17)</f>
-        <v>3.2</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -2386,7 +2436,7 @@
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>IF(ISBLANK(Steps!E18), "", Steps!E18)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -2395,7 +2445,7 @@
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>IF(ISBLANK(Steps!E19), "", Steps!E19)</f>
-        <v>4.0999999999999996</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -2404,7 +2454,7 @@
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>IF(ISBLANK(Steps!E20), "", Steps!E20)</f>
-        <v>4.2</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -2413,7 +2463,7 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>IF(ISBLANK(Steps!E21), "", Steps!E21)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -2422,7 +2472,7 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>IF(ISBLANK(Steps!E22), "", Steps!E22)</f>
-        <v>5.0999999999999996</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -2431,7 +2481,7 @@
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>IF(ISBLANK(Steps!E23), "", Steps!E23)</f>
-        <v>5.2</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -2440,7 +2490,7 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>IF(ISBLANK(Steps!E24), "", Steps!E24)</f>
-        <v>5.3</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -2449,7 +2499,7 @@
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>IF(ISBLANK(Steps!E25), "", Steps!E25)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -2458,7 +2508,7 @@
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>IF(ISBLANK(Steps!E26), "", Steps!E26)</f>
-        <v>6.1</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -2467,7 +2517,7 @@
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>IF(ISBLANK(Steps!E27), "", Steps!E27)</f>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -2476,7 +2526,7 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>IF(ISBLANK(Steps!E28), "", Steps!E28)</f>
-        <v>7.1</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -2485,7 +2535,7 @@
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>IF(ISBLANK(Steps!E29), "", Steps!E29)</f>
-        <v>7.2</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -2494,7 +2544,7 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>IF(ISBLANK(Steps!E30), "", Steps!E30)</f>
-        <v>7.3</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -2503,7 +2553,7 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>IF(ISBLANK(Steps!E31), "", Steps!E31)</f>
-        <v>7.4</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -2512,7 +2562,7 @@
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>IF(ISBLANK(Steps!E32), "", Steps!E32)</f>
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -2521,7 +2571,7 @@
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>IF(ISBLANK(Steps!E33), "", Steps!E33)</f>
-        <v>8.1</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -2530,7 +2580,7 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>IF(ISBLANK(Steps!E34), "", Steps!E34)</f>
-        <v>8.1999999999999993</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -2539,7 +2589,7 @@
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>IF(ISBLANK(Steps!E35), "", Steps!E35)</f>
-        <v>8.3000000000000007</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -2548,7 +2598,7 @@
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>IF(ISBLANK(Steps!E36), "", Steps!E36)</f>
-        <v>8.4</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -2557,7 +2607,7 @@
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>IF(ISBLANK(Steps!E37), "", Steps!E37)</f>
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -2566,7 +2616,7 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>IF(ISBLANK(Steps!E38), "", Steps!E38)</f>
-        <v>9.1</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -2575,7 +2625,7 @@
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>IF(ISBLANK(Steps!E39), "", Steps!E39)</f>
-        <v>9.1999999999999993</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -2584,7 +2634,7 @@
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>IF(ISBLANK(Steps!E40), "", Steps!E40)</f>
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -2593,7 +2643,7 @@
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>IF(ISBLANK(Steps!E41), "", Steps!E41)</f>
-        <v>10.1</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -2602,7 +2652,7 @@
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>IF(ISBLANK(Steps!E42), "", Steps!E42)</f>
-        <v>10.199999999999999</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -2611,7 +2661,7 @@
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>IF(ISBLANK(Steps!E43), "", Steps!E43)</f>
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -2620,7 +2670,7 @@
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>IF(ISBLANK(Steps!E44), "", Steps!E44)</f>
-        <v>11.1</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -2629,7 +2679,7 @@
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>IF(ISBLANK(Steps!E45), "", Steps!E45)</f>
-        <v>11.2</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -2638,7 +2688,7 @@
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>IF(ISBLANK(Steps!E46), "", Steps!E46)</f>
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -2647,7 +2697,7 @@
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>IF(ISBLANK(Steps!E47), "", Steps!E47)</f>
-        <v>12.1</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>46</v>
@@ -2656,7 +2706,7 @@
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>IF(ISBLANK(Steps!E48), "", Steps!E48)</f>
-        <v>12.2</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -2665,7 +2715,7 @@
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <f>IF(ISBLANK(Steps!E49), "", Steps!E49)</f>
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>48</v>
@@ -2674,7 +2724,7 @@
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>IF(ISBLANK(Steps!E50), "", Steps!E50)</f>
-        <v>13.1</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>49</v>
@@ -2683,7 +2733,7 @@
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>IF(ISBLANK(Steps!E51), "", Steps!E51)</f>
-        <v>13.2</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>50</v>
@@ -2692,7 +2742,7 @@
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <f>IF(ISBLANK(Steps!E52), "", Steps!E52)</f>
-        <v>13.3</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>51</v>

</xml_diff>